<commit_message>
Maximin selection algorithm implemented, new interface
</commit_message>
<xml_diff>
--- a/data/example-people.xlsx
+++ b/data/example-people.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -22,7 +22,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5117" uniqueCount="3044">
   <si>
-    <t xml:space="preserve">nationbuilder_id</t>
+    <t xml:space="preserve">id</t>
   </si>
   <si>
     <t xml:space="preserve">first_name</t>
@@ -9167,6 +9167,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -9255,10 +9256,10 @@
   <dimension ref="A1:Q301"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.96"/>
@@ -9268,7 +9269,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="7.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="6.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="10.88"/>

</xml_diff>